<commit_message>
added faction guide/zeta ranking and individual character pages
</commit_message>
<xml_diff>
--- a/src/data/teamdata.xlsx
+++ b/src/data/teamdata.xlsx
@@ -1,31 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxst\Projects\SWGOH_Companion_Site\swgoh-companion\src\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D8BF5D-A3FD-491B-9834-7D38D7B5AB8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="154">
   <si>
     <t>TEAM NAME</t>
   </si>
   <si>
     <t>TEAM COMPOSITION</t>
+  </si>
+  <si>
+    <t>OPTIONS</t>
   </si>
   <si>
     <t>GRAND ARENA OFFENSE</t>
@@ -71,6 +68,9 @@
     <t>GLLEIA, CAPTAINDROGAN, R2D2_LEGENDARY, BAZEMALBUS, MONMOTHMA</t>
   </si>
   <si>
+    <t>OLDBENKENOBI,CAPTAINREX,KANANJARRUSS3</t>
+  </si>
+  <si>
     <t>GALACTIC LEGEND</t>
   </si>
   <si>
@@ -81,6 +81,9 @@
     <t xml:space="preserve">GLAHSOKATANO, EZRAEXILE, PADAWANSABINE, HUYANG, GENERALSYNDULLA </t>
   </si>
   <si>
+    <t>FULCRUMAHSOKA</t>
+  </si>
+  <si>
     <t>Jedi Master Kenobi
 (JMK)</t>
   </si>
@@ -88,8 +91,16 @@
     <t>JEDIMASTERKENOBI,COMMANDERAHSOKA, AHSOKATANO,GENERALKENOBI,PADMEAMIDALA</t>
   </si>
   <si>
-    <t>Jabba the Hutt
-(JTH)</t>
+    <t>MACEWINDU</t>
+  </si>
+  <si>
+    <t>Jabba the Hutt</t>
+  </si>
+  <si>
+    <t>JABBATHEHUTT,BOUSHH,KRRSANTAN,UNDERCOVERLANDO, BOBAFETT</t>
+  </si>
+  <si>
+    <t>EMBO</t>
   </si>
   <si>
     <t>Lord Vader
@@ -99,10 +110,16 @@
     <t>LORDVADER,ADMIRALPIETT,MAULS7,VADER,ROYALGUARD</t>
   </si>
   <si>
+    <t>GRANDADMIRALTHRAWN,MOFFGIDEONS3,NINTHSISTER,THIRDSISTER,GRANDINQUISITOR</t>
+  </si>
+  <si>
     <t>Rey</t>
   </si>
   <si>
     <t>GLREY, BENSOLO</t>
+  </si>
+  <si>
+    <t>CALKESTIS</t>
   </si>
   <si>
     <t>Supreme Leader Kylo Ren
@@ -112,10 +129,16 @@
     <t>SUPREMELEADERKYLOREN,GENERALHUX,DARKREY,FOSITHTROOPER,KYLORENUNMASKED</t>
   </si>
   <si>
-    <t>Reva Inquisitors</t>
+    <t>FIRSTORDEROFFICERMALE, FIRSTORDEREXECUTIONER</t>
+  </si>
+  <si>
+    <t>Inquisitorius</t>
   </si>
   <si>
     <t>THIRDSISTER, GRANDINQUISITOR, SEVENTHSISTER,FIFTHBROTHER,EIGHTHBROTHER</t>
+  </si>
+  <si>
+    <t>SECONDSISTER,NINTHSISTER</t>
   </si>
   <si>
     <t xml:space="preserve">Jedi Master Luke Skywalker
@@ -126,6 +149,9 @@
     <t>GRANDMASTERLUKE, JEDIKNIGHTLUKE,HERMITYODA,JEDIKNIGHTCAL,JEDIKNIGHTREVAN</t>
   </si>
   <si>
+    <t>EZRAEXILE,GRANDMASTERYODA</t>
+  </si>
+  <si>
     <t>BESKAR</t>
   </si>
   <si>
@@ -137,6 +163,9 @@
     <t>SITHPALPATINE,WATTAMBOR</t>
   </si>
   <si>
+    <t>GEONOSIANBROODALPHA</t>
+  </si>
+  <si>
     <t>Great Mothers
 (GM)</t>
   </si>
@@ -144,11 +173,16 @@
     <t>GREATMOTHERS,MORGANELSBETH</t>
   </si>
   <si>
-    <t>Baylan Skoll
-(BS)</t>
-  </si>
-  <si>
-    <t>BAYLANSKOLL,SHINHATI,MARROK</t>
+    <t>NIGHTTROOPER,DEATHTROOPERPERIDEA</t>
+  </si>
+  <si>
+    <t>Baylan Skoll</t>
+  </si>
+  <si>
+    <t>BAYLANSKOLL,SHINHATI,MARROK,QIRA,HONDO</t>
+  </si>
+  <si>
+    <t>BOBAFETTSCION,DENGAR,CADBANE</t>
   </si>
   <si>
     <t>Starkiller
@@ -171,11 +205,20 @@
     <t>Bo Katan (Mand'alor)</t>
   </si>
   <si>
+    <t>MANDALORBOKATAN, THEMANDALORIANBESKARARMOR, PAZVIZSLA, IG12,BOKATAN</t>
+  </si>
+  <si>
+    <t>ARMORER,SABINEWRENS3,PADAWANSABINE</t>
+  </si>
+  <si>
     <t>Queen Amidala
 (Quadme)</t>
   </si>
   <si>
     <t>QUEENAMIDALA,PADAWANOBIWAN,MASTERQUIGON</t>
+  </si>
+  <si>
+    <t>GRANDMASTERYODA, SHAAKTI,BADBATCHECHO</t>
   </si>
   <si>
     <t>Taron Malicos
@@ -186,6 +229,9 @@
     <t>CEREJUNDA, TARONMALICOS, CALKESTIS,FULCRUMAHSOKA, KYLOREN</t>
   </si>
   <si>
+    <t>KYLORENUNMASKED</t>
+  </si>
+  <si>
     <t>Starkiller
 Grand Arena
 (SK)</t>
@@ -197,6 +243,9 @@
     <t>DARTHBANE,SITHASSASSIN</t>
   </si>
   <si>
+    <t>SITHTROOPER,COUNTDOOKU,MAUL, DARTHTALON</t>
+  </si>
+  <si>
     <t>Dark Trooper Moff Gideon
 (DTMG)</t>
   </si>
@@ -204,6 +253,9 @@
     <t>MOFFGIDEONS3, SCOUTTROOPER_V3,STORMTROOPER,DEATHTROOPER,MOFFGIDEONS1</t>
   </si>
   <si>
+    <t>TIEFIGHTERPILOT</t>
+  </si>
+  <si>
     <t xml:space="preserve">Darth Malgus
 </t>
   </si>
@@ -211,6 +263,9 @@
     <t>DARTHMALGUS, DARTHREVAN,DARTHMALAK,BASTILASHANDARK,SITHMARAUDER</t>
   </si>
   <si>
+    <t>SITHTROOPER</t>
+  </si>
+  <si>
     <t>Mauldalorians
 (Maul)</t>
   </si>
@@ -222,7 +277,10 @@
 with Captain Rex</t>
   </si>
   <si>
-    <t>GENERALSKYWALKER</t>
+    <t>GENERALSKYWALKER,CT7567,CT5555,ARCTROOPER501ST,CAPTAINREX</t>
+  </si>
+  <si>
+    <t>CT210408</t>
   </si>
   <si>
     <t>Sith Triumvirate
@@ -232,6 +290,9 @@
     <t>DARTHTRAYA,DARTHNIHILUS,SAVAGEOPRESS,DARTHTALON,SITHTROOPER</t>
   </si>
   <si>
+    <t>DARTHSION</t>
+  </si>
+  <si>
     <t>KYBER</t>
   </si>
   <si>
@@ -244,6 +305,9 @@
   <si>
     <t xml:space="preserve">Saw Gerrera w/ Luthen Rael
 </t>
+  </si>
+  <si>
+    <t>SAWGERRERA,LUTHENRAEL,KYLEKATARN,PAO,HOTHREBELSCOUT</t>
   </si>
   <si>
     <t>Captain Rex Phoenix</t>
@@ -257,17 +321,29 @@
 </t>
   </si>
   <si>
-    <t>GRIEVOUS</t>
+    <t>GRIEVOUS,STAP,B2SUPERBATTLEDROID,B1BATTLEDROIDV2,MAGNAGUARD</t>
+  </si>
+  <si>
+    <t>NUTEGUNRAY,DROIDEKA</t>
   </si>
   <si>
     <t>Zorii Resistance</t>
   </si>
   <si>
-    <t/>
+    <t>FINN,ZORIIBLISS_V2,POE,EPIXFINN,EPIXPOE,ROSETICO</t>
+  </si>
+  <si>
+    <t>ADMIRALHOLDO</t>
   </si>
   <si>
     <t>Nightsisters
 (NS)</t>
+  </si>
+  <si>
+    <t>MOTHERTALZIN, MERRIN, NIGHTSISTERZOMBIE, DAKA, ASAJVENTRESS</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t xml:space="preserve">General Anakin Skywalker 501st
@@ -322,9 +398,6 @@
 (ATF)</t>
   </si>
   <si>
-    <t>FULCRUMAHSOKA</t>
-  </si>
-  <si>
     <t>Kelleran Beq
 (KB)</t>
   </si>
@@ -474,69 +547,13 @@
   <si>
     <t>Old Republic
 (OR)</t>
-  </si>
-  <si>
-    <t>OPTIONS</t>
-  </si>
-  <si>
-    <t>OLDBENKENOBI,CAPTAINREX,KANANJARRUSS3</t>
-  </si>
-  <si>
-    <t>MACEWINDU</t>
-  </si>
-  <si>
-    <t>EMBO</t>
-  </si>
-  <si>
-    <t>JABBATHEHUTT,BOUSHH,KRRSANTAN,UNDERCOVERLANDO, BOBAFETT</t>
-  </si>
-  <si>
-    <t>GRANDADMIRALTHRAWN,MOFFGIDEONS3,NINTHSISTER,THIRDSISTER,GRANDINQUISITOR</t>
-  </si>
-  <si>
-    <t>CALKESTIS</t>
-  </si>
-  <si>
-    <t>FIRSTORDEROFFICER</t>
-  </si>
-  <si>
-    <t>SECONDSISTER,NINTHSISTER</t>
-  </si>
-  <si>
-    <t>EZRAEXILE</t>
-  </si>
-  <si>
-    <t>QIRA,HONDO</t>
-  </si>
-  <si>
-    <t>NIGHTTROOPER,DEATHTROOPERPERIDEA</t>
-  </si>
-  <si>
-    <t>GRANDMASTERYODA, SHAAKTI,BADBATCHECHO</t>
-  </si>
-  <si>
-    <t>KYLORENUNMASKED</t>
-  </si>
-  <si>
-    <t>SITHTROOPER,COUNTDOOKU,MAUL, DARTHTALON</t>
-  </si>
-  <si>
-    <t>SITHTROOPER</t>
-  </si>
-  <si>
-    <t>TIEFIGHTERPILOT</t>
-  </si>
-  <si>
-    <t>DARTHSION</t>
-  </si>
-  <si>
-    <t>NUTEGUNRAY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -548,7 +565,7 @@
     <font>
       <b/>
       <sz val="14"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFffffff"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -573,11 +590,11 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFffffff"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -593,7 +610,7 @@
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
@@ -602,13 +619,13 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </left>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
@@ -617,13 +634,13 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </left>
       <right style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </right>
       <top style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
@@ -638,53 +655,40 @@
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </left>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </left>
       <right style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </right>
       <top style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFC6C6C6"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FFC6C6C6"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
+        <color rgb="FFc6c6c6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -693,159 +697,114 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="25">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FFC6C6C6"/>
-        </left>
-        <right style="medium">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFC6C6C6"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:O81" totalsRowShown="0">
-  <autoFilter ref="A1:O81" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:O81" displayName="Table1" name="Table1" id="1" totalsRowShown="0">
+  <autoFilter ref="A1:O81"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TEAM NAME"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="TEAM COMPOSITION"/>
-    <tableColumn id="16" xr3:uid="{305666D1-1225-4F34-90E7-A31CE101C440}" name="OPTIONS" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="GRAND ARENA OFFENSE"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="GRAND ARENA DEFENSE"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="GRAND ARENA OVERALL"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="OVERALL GRAND ARENA RANK"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="GAC OMICRONS REQUIRED"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="TERRITORY WARS OFFENSE"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="TERRITORY WARS DEFENSE"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="TERRITORY WARS OVERALL"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="OVERALL TERRITORY WARS RANK"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="TW OMICRONS REQUIRED"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="TOTAL OVERALL SCORE"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="OVERALL RANK"/>
+    <tableColumn name="TEAM NAME" id="1"/>
+    <tableColumn name="TEAM COMPOSITION" id="2"/>
+    <tableColumn name="OPTIONS" id="3"/>
+    <tableColumn name="GRAND ARENA OFFENSE" id="4"/>
+    <tableColumn name="GRAND ARENA DEFENSE" id="5"/>
+    <tableColumn name="GRAND ARENA OVERALL" id="6"/>
+    <tableColumn name="OVERALL GRAND ARENA RANK" id="7"/>
+    <tableColumn name="GAC OMICRONS REQUIRED" id="8"/>
+    <tableColumn name="TERRITORY WARS OFFENSE" id="9"/>
+    <tableColumn name="TERRITORY WARS DEFENSE" id="10"/>
+    <tableColumn name="TERRITORY WARS OVERALL" id="11"/>
+    <tableColumn name="OVERALL TERRITORY WARS RANK" id="12"/>
+    <tableColumn name="TW OMICRONS REQUIRED" id="13"/>
+    <tableColumn name="TOTAL OVERALL SCORE" id="14"/>
+    <tableColumn name="OVERALL RANK" id="15"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight1" showColumnStripes="0" showRowStripes="1" showLastColumn="0" showFirstColumn="0"/>
 </table>
 </file>
 
@@ -854,10 +813,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -895,71 +854,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -987,7 +946,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -1010,11 +969,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -1023,13 +982,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1039,7 +998,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1048,7 +1007,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1057,7 +1016,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1065,10 +1024,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -1133,36 +1092,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:O81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.42578125" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="31.7109375" style="23" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.5703125" style="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="21" width="49.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="22" width="54.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="22" width="39.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="23" width="25.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="23" width="23.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="23" width="22.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="24" width="28.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="23" width="28.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="23" width="26.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="23" width="28.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="23" width="28.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="24" width="31.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="23" width="22.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="23" width="23.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="24" width="24.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="55.5" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1170,54 +1127,54 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>127</v>
+        <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="33.75">
       <c r="A2" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>128</v>
+        <v>17</v>
       </c>
       <c r="D2" s="8">
         <v>10</v>
@@ -1229,7 +1186,7 @@
         <v>9.5</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H2" s="8">
         <v>0</v>
@@ -1244,7 +1201,7 @@
         <v>9.5</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="M2" s="8">
         <v>0</v>
@@ -1253,18 +1210,18 @@
         <v>9.5</v>
       </c>
       <c r="O2" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="47.25">
       <c r="A3" s="6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>86</v>
+        <v>21</v>
       </c>
       <c r="D3" s="8">
         <v>10</v>
@@ -1276,7 +1233,7 @@
         <v>9.5</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H3" s="8">
         <v>2</v>
@@ -1291,7 +1248,7 @@
         <v>9.5</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="M3" s="8">
         <v>1</v>
@@ -1300,18 +1257,18 @@
         <v>9.5</v>
       </c>
       <c r="O3" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="47.25">
       <c r="A4" s="6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>129</v>
+        <v>24</v>
       </c>
       <c r="D4" s="8">
         <v>9</v>
@@ -1323,7 +1280,7 @@
         <v>8.5</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H4" s="8">
         <v>0</v>
@@ -1338,7 +1295,7 @@
         <v>9</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="M4" s="8">
         <v>0</v>
@@ -1347,18 +1304,18 @@
         <v>8.75</v>
       </c>
       <c r="O4" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="33.75">
       <c r="A5" s="6" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>131</v>
+        <v>26</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>130</v>
+        <v>27</v>
       </c>
       <c r="D5" s="8">
         <v>9</v>
@@ -1370,7 +1327,7 @@
         <v>8.5</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H5" s="8">
         <v>0</v>
@@ -1385,7 +1342,7 @@
         <v>9</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="M5" s="8">
         <v>1</v>
@@ -1394,18 +1351,18 @@
         <v>8.75</v>
       </c>
       <c r="O5" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="47.25">
       <c r="A6" s="6" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>132</v>
+        <v>30</v>
       </c>
       <c r="D6" s="8">
         <v>9</v>
@@ -1417,7 +1374,7 @@
         <v>8.5</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H6" s="8">
         <v>0</v>
@@ -1432,7 +1389,7 @@
         <v>9</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="M6" s="8">
         <v>0</v>
@@ -1441,18 +1398,18 @@
         <v>8.75</v>
       </c>
       <c r="O6" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
       <c r="A7" s="6" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>133</v>
+        <v>33</v>
       </c>
       <c r="D7" s="8">
         <v>8</v>
@@ -1464,7 +1421,7 @@
         <v>8</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H7" s="8">
         <v>1</v>
@@ -1479,7 +1436,7 @@
         <v>8.5</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="M7" s="8">
         <v>0</v>
@@ -1488,18 +1445,18 @@
         <v>8.25</v>
       </c>
       <c r="O7" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="33.75">
       <c r="A8" s="6" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>134</v>
+        <v>36</v>
       </c>
       <c r="D8" s="8">
         <v>9</v>
@@ -1511,7 +1468,7 @@
         <v>8.5</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H8" s="8">
         <v>0</v>
@@ -1526,7 +1483,7 @@
         <v>8</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="M8" s="8">
         <v>0</v>
@@ -1535,18 +1492,18 @@
         <v>8.25</v>
       </c>
       <c r="O8" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="47.25">
       <c r="A9" s="6" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>135</v>
+        <v>39</v>
       </c>
       <c r="D9" s="8">
         <v>9</v>
@@ -1558,7 +1515,7 @@
         <v>8</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H9" s="8">
         <v>1</v>
@@ -1573,7 +1530,7 @@
         <v>8</v>
       </c>
       <c r="L9" s="10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="M9" s="8">
         <v>2</v>
@@ -1582,18 +1539,18 @@
         <v>8</v>
       </c>
       <c r="O9" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="47.25">
       <c r="A10" s="6" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>136</v>
+        <v>42</v>
       </c>
       <c r="D10" s="8">
         <v>8</v>
@@ -1605,7 +1562,7 @@
         <v>7.5</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="H10" s="8">
         <v>0</v>
@@ -1620,7 +1577,7 @@
         <v>7.5</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="M10" s="8">
         <v>0</v>
@@ -1629,17 +1586,19 @@
         <v>7.5</v>
       </c>
       <c r="O10" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="33.75">
       <c r="A11" s="6" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="7"/>
+        <v>45</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="D11" s="8">
         <v>8</v>
       </c>
@@ -1650,7 +1609,7 @@
         <v>7.5</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="H11" s="8">
         <v>1</v>
@@ -1665,7 +1624,7 @@
         <v>7.5</v>
       </c>
       <c r="L11" s="10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="M11" s="8">
         <v>0</v>
@@ -1674,18 +1633,18 @@
         <v>7.5</v>
       </c>
       <c r="O11" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="33.75">
       <c r="A12" s="6" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>138</v>
+        <v>49</v>
       </c>
       <c r="D12" s="8">
         <v>7</v>
@@ -1697,7 +1656,7 @@
         <v>6.5</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="H12" s="8">
         <v>1</v>
@@ -1712,7 +1671,7 @@
         <v>8</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="M12" s="8">
         <v>1</v>
@@ -1721,18 +1680,18 @@
         <v>7.25</v>
       </c>
       <c r="O12" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25">
       <c r="A13" s="6" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>137</v>
+        <v>52</v>
       </c>
       <c r="D13" s="8">
         <v>8</v>
@@ -1744,7 +1703,7 @@
         <v>7.5</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="H13" s="8">
         <v>2</v>
@@ -1759,7 +1718,7 @@
         <v>6.5</v>
       </c>
       <c r="L13" s="10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="M13" s="8">
         <v>1</v>
@@ -1768,31 +1727,31 @@
         <v>7</v>
       </c>
       <c r="O13" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="47.25">
       <c r="A14" s="6" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="8" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="I14" s="8">
         <v>7</v>
@@ -1804,7 +1763,7 @@
         <v>7</v>
       </c>
       <c r="L14" s="10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="M14" s="8">
         <v>1</v>
@@ -1813,15 +1772,15 @@
         <v>7</v>
       </c>
       <c r="O14" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="47.25">
       <c r="A15" s="6" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="8">
@@ -1834,7 +1793,7 @@
         <v>7</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="H15" s="8">
         <v>2</v>
@@ -1849,7 +1808,7 @@
         <v>7</v>
       </c>
       <c r="L15" s="10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="M15" s="8">
         <v>1</v>
@@ -1858,15 +1817,19 @@
         <v>7</v>
       </c>
       <c r="O15" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="47.25">
       <c r="A16" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
+        <v>58</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D16" s="8">
         <v>7</v>
       </c>
@@ -1877,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="H16" s="8">
         <v>1</v>
@@ -1892,7 +1855,7 @@
         <v>7</v>
       </c>
       <c r="L16" s="10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="M16" s="8">
         <v>0</v>
@@ -1901,18 +1864,18 @@
         <v>7</v>
       </c>
       <c r="O16" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="33.75">
       <c r="A17" s="6" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>139</v>
+        <v>63</v>
       </c>
       <c r="D17" s="8">
         <v>7</v>
@@ -1924,7 +1887,7 @@
         <v>7.5</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="H17" s="8">
         <v>2</v>
@@ -1939,7 +1902,7 @@
         <v>6.5</v>
       </c>
       <c r="L17" s="10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="M17" s="8">
         <v>1</v>
@@ -1948,18 +1911,18 @@
         <v>7</v>
       </c>
       <c r="O17" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="47.25">
       <c r="A18" s="6" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>140</v>
+        <v>66</v>
       </c>
       <c r="D18" s="8">
         <v>7</v>
@@ -1971,7 +1934,7 @@
         <v>7.5</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="H18" s="8">
         <v>4</v>
@@ -1986,7 +1949,7 @@
         <v>6.5</v>
       </c>
       <c r="L18" s="10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="M18" s="8">
         <v>2</v>
@@ -1995,15 +1958,15 @@
         <v>7</v>
       </c>
       <c r="O18" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="47.25">
       <c r="A19" s="6" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="8">
@@ -2016,42 +1979,42 @@
         <v>7</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="H19" s="8">
         <v>1</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="L19" s="10" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="M19" s="8" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="N19" s="8">
         <v>7</v>
       </c>
       <c r="O19" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="33.75">
       <c r="A20" s="6" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>141</v>
+        <v>70</v>
       </c>
       <c r="D20" s="8">
         <v>10</v>
@@ -2063,7 +2026,7 @@
         <v>6.5</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="H20" s="8">
         <v>1</v>
@@ -2078,7 +2041,7 @@
         <v>7</v>
       </c>
       <c r="L20" s="10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="M20" s="8">
         <v>0</v>
@@ -2087,18 +2050,18 @@
         <v>6.75</v>
       </c>
       <c r="O20" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="47.25">
       <c r="A21" s="6" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>143</v>
+        <v>73</v>
       </c>
       <c r="D21" s="8">
         <v>6</v>
@@ -2110,7 +2073,7 @@
         <v>6</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="H21" s="8">
         <v>0</v>
@@ -2125,7 +2088,7 @@
         <v>7.5</v>
       </c>
       <c r="L21" s="10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="M21" s="8">
         <v>2</v>
@@ -2134,18 +2097,18 @@
         <v>6.75</v>
       </c>
       <c r="O21" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="47.25">
       <c r="A22" s="6" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>142</v>
+        <v>76</v>
       </c>
       <c r="D22" s="8">
         <v>7</v>
@@ -2157,7 +2120,7 @@
         <v>6.5</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="H22" s="8">
         <v>2</v>
@@ -2172,7 +2135,7 @@
         <v>6.5</v>
       </c>
       <c r="L22" s="10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="M22" s="8">
         <v>0</v>
@@ -2181,15 +2144,15 @@
         <v>6.5</v>
       </c>
       <c r="O22" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="33.75">
       <c r="A23" s="6" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="8">
@@ -2202,7 +2165,7 @@
         <v>6</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="H23" s="8">
         <v>0</v>
@@ -2217,7 +2180,7 @@
         <v>6.5</v>
       </c>
       <c r="L23" s="10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="M23" s="8">
         <v>0</v>
@@ -2226,17 +2189,19 @@
         <v>6.25</v>
       </c>
       <c r="O23" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="33.75">
       <c r="A24" s="6" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C24" s="7"/>
+        <v>80</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>81</v>
+      </c>
       <c r="D24" s="8">
         <v>6</v>
       </c>
@@ -2247,7 +2212,7 @@
         <v>6</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="H24" s="8">
         <v>0</v>
@@ -2262,7 +2227,7 @@
         <v>6</v>
       </c>
       <c r="L24" s="10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="M24" s="8">
         <v>0</v>
@@ -2271,18 +2236,18 @@
         <v>6</v>
       </c>
       <c r="O24" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="33.75">
       <c r="A25" s="6" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>144</v>
+        <v>84</v>
       </c>
       <c r="D25" s="8">
         <v>6</v>
@@ -2294,7 +2259,7 @@
         <v>6</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="H25" s="8">
         <v>2</v>
@@ -2309,7 +2274,7 @@
         <v>4.5</v>
       </c>
       <c r="L25" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="M25" s="8">
         <v>0</v>
@@ -2318,15 +2283,15 @@
         <v>5.25</v>
       </c>
       <c r="O25" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="33.75">
       <c r="A26" s="6" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="8">
@@ -2339,7 +2304,7 @@
         <v>5.5</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H26" s="8">
         <v>1</v>
@@ -2354,7 +2319,7 @@
         <v>5</v>
       </c>
       <c r="L26" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="M26" s="8">
         <v>0</v>
@@ -2363,14 +2328,16 @@
         <v>5.25</v>
       </c>
       <c r="O26" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="20.25">
       <c r="A27" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B27" s="7"/>
+        <v>88</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>89</v>
+      </c>
       <c r="C27" s="7"/>
       <c r="D27" s="8">
         <v>6</v>
@@ -2382,7 +2349,7 @@
         <v>6.5</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H27" s="8">
         <v>2</v>
@@ -2397,7 +2364,7 @@
         <v>4</v>
       </c>
       <c r="L27" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="M27" s="8">
         <v>0</v>
@@ -2406,12 +2373,12 @@
         <v>5.25</v>
       </c>
       <c r="O27" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="20.25">
       <c r="A28" s="6" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -2425,7 +2392,7 @@
         <v>4.5</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H28" s="8">
         <v>1</v>
@@ -2440,7 +2407,7 @@
         <v>5.5</v>
       </c>
       <c r="L28" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="M28" s="8">
         <v>1</v>
@@ -2449,12 +2416,12 @@
         <v>5</v>
       </c>
       <c r="O28" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="6" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -2468,7 +2435,7 @@
         <v>4.5</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H29" s="8">
         <v>0</v>
@@ -2483,7 +2450,7 @@
         <v>5.5</v>
       </c>
       <c r="L29" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="M29" s="8">
         <v>0</v>
@@ -2492,18 +2459,18 @@
         <v>5</v>
       </c>
       <c r="O29" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="6" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>145</v>
+        <v>94</v>
       </c>
       <c r="D30" s="8">
         <v>5</v>
@@ -2515,7 +2482,7 @@
         <v>4.5</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H30" s="8">
         <v>1</v>
@@ -2530,7 +2497,7 @@
         <v>5.5</v>
       </c>
       <c r="L30" s="10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="M30" s="8">
         <v>1</v>
@@ -2539,17 +2506,19 @@
         <v>5</v>
       </c>
       <c r="O30" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B31" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="C31" s="12"/>
+        <v>95</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>97</v>
+      </c>
       <c r="D31" s="8">
         <v>6</v>
       </c>
@@ -2560,7 +2529,7 @@
         <v>5</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="H31" s="8">
         <v>1</v>
@@ -2575,7 +2544,7 @@
         <v>5</v>
       </c>
       <c r="L31" s="10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="M31" s="8">
         <v>0</v>
@@ -2584,15 +2553,19 @@
         <v>5</v>
       </c>
       <c r="O31" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
+        <v>98</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>100</v>
+      </c>
       <c r="D32" s="8">
         <v>5</v>
       </c>
@@ -2603,7 +2576,7 @@
         <v>5</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H32" s="8">
         <v>1</v>
@@ -2618,7 +2591,7 @@
         <v>5</v>
       </c>
       <c r="L32" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="M32" s="8">
         <v>0</v>
@@ -2627,12 +2600,12 @@
         <v>5</v>
       </c>
       <c r="O32" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="6" t="s">
-        <v>73</v>
+        <v>101</v>
       </c>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -2646,7 +2619,7 @@
         <v>5</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H33" s="8">
         <v>0</v>
@@ -2661,7 +2634,7 @@
         <v>5</v>
       </c>
       <c r="L33" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="M33" s="8">
         <v>0</v>
@@ -2670,12 +2643,12 @@
         <v>5</v>
       </c>
       <c r="O33" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="6" t="s">
-        <v>74</v>
+        <v>102</v>
       </c>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
@@ -2689,7 +2662,7 @@
         <v>5</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H34" s="8">
         <v>0</v>
@@ -2704,7 +2677,7 @@
         <v>5</v>
       </c>
       <c r="L34" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="M34" s="8">
         <v>0</v>
@@ -2713,12 +2686,12 @@
         <v>5</v>
       </c>
       <c r="O34" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="6" t="s">
-        <v>75</v>
+        <v>103</v>
       </c>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
@@ -2732,7 +2705,7 @@
         <v>5.5</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H35" s="8">
         <v>2</v>
@@ -2747,7 +2720,7 @@
         <v>4.5</v>
       </c>
       <c r="L35" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="M35" s="8">
         <v>0</v>
@@ -2756,12 +2729,12 @@
         <v>5</v>
       </c>
       <c r="O35" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
       <c r="A36" s="6" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -2775,36 +2748,36 @@
         <v>5</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H36" s="8">
         <v>1</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="J36" s="8" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="K36" s="8" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="L36" s="10" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="M36" s="8" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="N36" s="8">
         <v>5</v>
       </c>
       <c r="O36" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
       <c r="A37" s="6" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
@@ -2818,36 +2791,36 @@
         <v>5</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H37" s="8">
         <v>1</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="J37" s="8" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="K37" s="8" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="L37" s="10" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="M37" s="8" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="N37" s="8">
         <v>5</v>
       </c>
       <c r="O37" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
       <c r="A38" s="6" t="s">
-        <v>78</v>
+        <v>106</v>
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
@@ -2861,7 +2834,7 @@
         <v>5</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H38" s="8">
         <v>0</v>
@@ -2876,7 +2849,7 @@
         <v>5</v>
       </c>
       <c r="L38" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="M38" s="8">
         <v>0</v>
@@ -2885,12 +2858,12 @@
         <v>5</v>
       </c>
       <c r="O38" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
       <c r="A39" s="6" t="s">
-        <v>79</v>
+        <v>107</v>
       </c>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
@@ -2898,87 +2871,87 @@
         <v>5</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="F39" s="8">
         <v>5</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H39" s="8">
         <v>1</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="J39" s="8" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="K39" s="8" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="L39" s="10" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="M39" s="8" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="N39" s="8">
         <v>5</v>
       </c>
       <c r="O39" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
       <c r="A40" s="6" t="s">
-        <v>80</v>
+        <v>108</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
       <c r="C40" s="7"/>
       <c r="D40" s="8">
         <v>5</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="F40" s="8">
         <v>5</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H40" s="8">
         <v>1</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="J40" s="8" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="K40" s="8" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="L40" s="10" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="M40" s="8" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="N40" s="8">
         <v>5</v>
       </c>
       <c r="O40" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
       <c r="A41" s="6" t="s">
-        <v>82</v>
+        <v>110</v>
       </c>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
@@ -2992,7 +2965,7 @@
         <v>4</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H41" s="8">
         <v>0</v>
@@ -3007,7 +2980,7 @@
         <v>6</v>
       </c>
       <c r="L41" s="10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="M41" s="8">
         <v>3</v>
@@ -3016,12 +2989,12 @@
         <v>5</v>
       </c>
       <c r="O41" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
       <c r="A42" s="6" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
@@ -3035,7 +3008,7 @@
         <v>3.5</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="H42" s="8">
         <v>0</v>
@@ -3050,7 +3023,7 @@
         <v>6.5</v>
       </c>
       <c r="L42" s="10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="M42" s="8">
         <v>2</v>
@@ -3059,28 +3032,28 @@
         <v>5</v>
       </c>
       <c r="O42" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
       <c r="A43" s="6" t="s">
-        <v>85</v>
+        <v>113</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>86</v>
+        <v>21</v>
       </c>
       <c r="C43" s="7"/>
       <c r="D43" s="8" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="H43" s="8">
         <v>0</v>
@@ -3089,13 +3062,13 @@
         <v>5</v>
       </c>
       <c r="J43" s="8" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="K43" s="8">
         <v>5</v>
       </c>
       <c r="L43" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="M43" s="8">
         <v>1</v>
@@ -3104,12 +3077,12 @@
         <v>5</v>
       </c>
       <c r="O43" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
       <c r="A44" s="6" t="s">
-        <v>87</v>
+        <v>114</v>
       </c>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
@@ -3123,7 +3096,7 @@
         <v>4</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H44" s="8">
         <v>0</v>
@@ -3138,7 +3111,7 @@
         <v>5.5</v>
       </c>
       <c r="L44" s="10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="M44" s="8">
         <v>1</v>
@@ -3147,12 +3120,12 @@
         <v>4.75</v>
       </c>
       <c r="O44" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
       <c r="A45" s="6" t="s">
-        <v>88</v>
+        <v>115</v>
       </c>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
@@ -3166,7 +3139,7 @@
         <v>4</v>
       </c>
       <c r="G45" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H45" s="8">
         <v>0</v>
@@ -3181,7 +3154,7 @@
         <v>5.5</v>
       </c>
       <c r="L45" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="M45" s="8">
         <v>0</v>
@@ -3190,12 +3163,12 @@
         <v>4.75</v>
       </c>
       <c r="O45" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
       <c r="A46" s="6" t="s">
-        <v>89</v>
+        <v>116</v>
       </c>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
@@ -3209,7 +3182,7 @@
         <v>4.5</v>
       </c>
       <c r="G46" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H46" s="8">
         <v>0</v>
@@ -3224,7 +3197,7 @@
         <v>4.5</v>
       </c>
       <c r="L46" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="M46" s="8">
         <v>0</v>
@@ -3233,12 +3206,12 @@
         <v>4.5</v>
       </c>
       <c r="O46" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
       <c r="A47" s="6" t="s">
-        <v>90</v>
+        <v>117</v>
       </c>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
@@ -3252,7 +3225,7 @@
         <v>4.5</v>
       </c>
       <c r="G47" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H47" s="8">
         <v>0</v>
@@ -3267,7 +3240,7 @@
         <v>4.5</v>
       </c>
       <c r="L47" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="M47" s="8">
         <v>0</v>
@@ -3276,12 +3249,12 @@
         <v>4.5</v>
       </c>
       <c r="O47" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
       <c r="A48" s="6" t="s">
-        <v>91</v>
+        <v>118</v>
       </c>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
@@ -3295,7 +3268,7 @@
         <v>4.5</v>
       </c>
       <c r="G48" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H48" s="8">
         <v>0</v>
@@ -3310,7 +3283,7 @@
         <v>4.5</v>
       </c>
       <c r="L48" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="M48" s="8">
         <v>0</v>
@@ -3319,12 +3292,12 @@
         <v>4.5</v>
       </c>
       <c r="O48" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
       <c r="A49" s="6" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
@@ -3338,7 +3311,7 @@
         <v>5</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H49" s="8">
         <v>1</v>
@@ -3353,7 +3326,7 @@
         <v>4</v>
       </c>
       <c r="L49" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="M49" s="8">
         <v>0</v>
@@ -3362,12 +3335,12 @@
         <v>4.5</v>
       </c>
       <c r="O49" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
       <c r="A50" s="6" t="s">
-        <v>93</v>
+        <v>120</v>
       </c>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
@@ -3381,7 +3354,7 @@
         <v>4.5</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H50" s="8">
         <v>0</v>
@@ -3396,7 +3369,7 @@
         <v>4.5</v>
       </c>
       <c r="L50" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="M50" s="8">
         <v>0</v>
@@ -3405,12 +3378,12 @@
         <v>4.5</v>
       </c>
       <c r="O50" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
       <c r="A51" s="6" t="s">
-        <v>94</v>
+        <v>121</v>
       </c>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
@@ -3424,7 +3397,7 @@
         <v>4</v>
       </c>
       <c r="G51" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H51" s="8">
         <v>1</v>
@@ -3439,7 +3412,7 @@
         <v>5</v>
       </c>
       <c r="L51" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="M51" s="8">
         <v>2</v>
@@ -3448,12 +3421,12 @@
         <v>4.5</v>
       </c>
       <c r="O51" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
       <c r="A52" s="6" t="s">
-        <v>95</v>
+        <v>122</v>
       </c>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
@@ -3467,7 +3440,7 @@
         <v>4</v>
       </c>
       <c r="G52" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H52" s="8">
         <v>0</v>
@@ -3482,7 +3455,7 @@
         <v>4.5</v>
       </c>
       <c r="L52" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="M52" s="8">
         <v>0</v>
@@ -3491,12 +3464,12 @@
         <v>4.25</v>
       </c>
       <c r="O52" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
       <c r="A53" s="6" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
@@ -3510,7 +3483,7 @@
         <v>3</v>
       </c>
       <c r="G53" s="10" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="H53" s="8">
         <v>0</v>
@@ -3525,7 +3498,7 @@
         <v>5.5</v>
       </c>
       <c r="L53" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="M53" s="8">
         <v>1</v>
@@ -3534,12 +3507,12 @@
         <v>4.25</v>
       </c>
       <c r="O53" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
       <c r="A54" s="6" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
@@ -3553,7 +3526,7 @@
         <v>5</v>
       </c>
       <c r="G54" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H54" s="8">
         <v>1</v>
@@ -3568,7 +3541,7 @@
         <v>3.5</v>
       </c>
       <c r="L54" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="M54" s="8">
         <v>0</v>
@@ -3577,12 +3550,12 @@
         <v>4.25</v>
       </c>
       <c r="O54" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
       <c r="A55" s="6" t="s">
-        <v>98</v>
+        <v>125</v>
       </c>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
@@ -3596,7 +3569,7 @@
         <v>3.5</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H55" s="8">
         <v>0</v>
@@ -3611,7 +3584,7 @@
         <v>4.5</v>
       </c>
       <c r="L55" s="10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="M55" s="8">
         <v>1</v>
@@ -3620,12 +3593,12 @@
         <v>4</v>
       </c>
       <c r="O55" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
       <c r="A56" s="6" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
@@ -3639,7 +3612,7 @@
         <v>4</v>
       </c>
       <c r="G56" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H56" s="8">
         <v>0</v>
@@ -3654,7 +3627,7 @@
         <v>4</v>
       </c>
       <c r="L56" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="M56" s="8">
         <v>0</v>
@@ -3663,12 +3636,12 @@
         <v>4</v>
       </c>
       <c r="O56" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
       <c r="A57" s="6" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
@@ -3682,7 +3655,7 @@
         <v>4</v>
       </c>
       <c r="G57" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H57" s="8">
         <v>1</v>
@@ -3697,7 +3670,7 @@
         <v>4</v>
       </c>
       <c r="L57" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="M57" s="8">
         <v>0</v>
@@ -3706,12 +3679,12 @@
         <v>4</v>
       </c>
       <c r="O57" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
       <c r="A58" s="6" t="s">
-        <v>101</v>
+        <v>128</v>
       </c>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
@@ -3725,7 +3698,7 @@
         <v>4</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H58" s="8">
         <v>0</v>
@@ -3740,7 +3713,7 @@
         <v>4</v>
       </c>
       <c r="L58" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="M58" s="8">
         <v>0</v>
@@ -3749,12 +3722,12 @@
         <v>4</v>
       </c>
       <c r="O58" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
       <c r="A59" s="6" t="s">
-        <v>102</v>
+        <v>129</v>
       </c>
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
@@ -3768,7 +3741,7 @@
         <v>4</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H59" s="8">
         <v>0</v>
@@ -3783,7 +3756,7 @@
         <v>4</v>
       </c>
       <c r="L59" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="M59" s="8">
         <v>0</v>
@@ -3792,12 +3765,12 @@
         <v>4</v>
       </c>
       <c r="O59" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
       <c r="A60" s="6" t="s">
-        <v>103</v>
+        <v>130</v>
       </c>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
@@ -3811,7 +3784,7 @@
         <v>2.5</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="H60" s="8">
         <v>0</v>
@@ -3826,7 +3799,7 @@
         <v>5</v>
       </c>
       <c r="L60" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="M60" s="8">
         <v>1</v>
@@ -3835,12 +3808,12 @@
         <v>3.75</v>
       </c>
       <c r="O60" s="11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
       <c r="A61" s="6" t="s">
-        <v>105</v>
+        <v>132</v>
       </c>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
@@ -3854,7 +3827,7 @@
         <v>4</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H61" s="8">
         <v>1</v>
@@ -3869,7 +3842,7 @@
         <v>3.5</v>
       </c>
       <c r="L61" s="10" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="M61" s="8">
         <v>0</v>
@@ -3878,12 +3851,12 @@
         <v>3.75</v>
       </c>
       <c r="O61" s="11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
       <c r="A62" s="6" t="s">
-        <v>106</v>
+        <v>133</v>
       </c>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
@@ -3897,7 +3870,7 @@
         <v>4.5</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H62" s="8">
         <v>0</v>
@@ -3912,7 +3885,7 @@
         <v>3</v>
       </c>
       <c r="L62" s="10" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="M62" s="8">
         <v>0</v>
@@ -3921,12 +3894,12 @@
         <v>3.75</v>
       </c>
       <c r="O62" s="11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
       <c r="A63" s="6" t="s">
-        <v>107</v>
+        <v>134</v>
       </c>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
@@ -3940,7 +3913,7 @@
         <v>3.5</v>
       </c>
       <c r="G63" s="10" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="H63" s="8">
         <v>0</v>
@@ -3955,7 +3928,7 @@
         <v>3.5</v>
       </c>
       <c r="L63" s="10" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="M63" s="8">
         <v>0</v>
@@ -3964,12 +3937,12 @@
         <v>3.5</v>
       </c>
       <c r="O63" s="11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
       <c r="A64" s="6" t="s">
-        <v>108</v>
+        <v>135</v>
       </c>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
@@ -3983,7 +3956,7 @@
         <v>3.5</v>
       </c>
       <c r="G64" s="10" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="H64" s="8">
         <v>0</v>
@@ -3998,7 +3971,7 @@
         <v>3.5</v>
       </c>
       <c r="L64" s="10" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="M64" s="8">
         <v>0</v>
@@ -4007,12 +3980,12 @@
         <v>3.5</v>
       </c>
       <c r="O64" s="11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="65" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
       <c r="A65" s="6" t="s">
-        <v>109</v>
+        <v>136</v>
       </c>
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
@@ -4026,7 +3999,7 @@
         <v>3.5</v>
       </c>
       <c r="G65" s="10" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="H65" s="8">
         <v>0</v>
@@ -4041,7 +4014,7 @@
         <v>3.5</v>
       </c>
       <c r="L65" s="10" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="M65" s="8">
         <v>0</v>
@@ -4050,12 +4023,12 @@
         <v>3.5</v>
       </c>
       <c r="O65" s="11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="66" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
       <c r="A66" s="6" t="s">
-        <v>110</v>
+        <v>137</v>
       </c>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
@@ -4069,7 +4042,7 @@
         <v>3.5</v>
       </c>
       <c r="G66" s="10" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="H66" s="8">
         <v>0</v>
@@ -4084,7 +4057,7 @@
         <v>3.5</v>
       </c>
       <c r="L66" s="10" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="M66" s="8">
         <v>0</v>
@@ -4093,12 +4066,12 @@
         <v>3.5</v>
       </c>
       <c r="O66" s="11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="67" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
       <c r="A67" s="6" t="s">
-        <v>111</v>
+        <v>138</v>
       </c>
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
@@ -4112,7 +4085,7 @@
         <v>3.5</v>
       </c>
       <c r="G67" s="10" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="H67" s="8">
         <v>0</v>
@@ -4127,7 +4100,7 @@
         <v>3.5</v>
       </c>
       <c r="L67" s="10" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="M67" s="8">
         <v>0</v>
@@ -4136,12 +4109,12 @@
         <v>3.5</v>
       </c>
       <c r="O67" s="11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="68" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
       <c r="A68" s="6" t="s">
-        <v>112</v>
+        <v>139</v>
       </c>
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
@@ -4155,7 +4128,7 @@
         <v>3.5</v>
       </c>
       <c r="G68" s="10" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="H68" s="8">
         <v>1</v>
@@ -4170,7 +4143,7 @@
         <v>3</v>
       </c>
       <c r="L68" s="10" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="M68" s="8">
         <v>1</v>
@@ -4179,12 +4152,12 @@
         <v>3.25</v>
       </c>
       <c r="O68" s="11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
       <c r="A69" s="6" t="s">
-        <v>113</v>
+        <v>140</v>
       </c>
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
@@ -4198,7 +4171,7 @@
         <v>3.5</v>
       </c>
       <c r="G69" s="10" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="H69" s="8">
         <v>1</v>
@@ -4213,7 +4186,7 @@
         <v>3</v>
       </c>
       <c r="L69" s="10" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="M69" s="8">
         <v>0</v>
@@ -4222,12 +4195,12 @@
         <v>3.25</v>
       </c>
       <c r="O69" s="11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="70" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
       <c r="A70" s="6" t="s">
-        <v>114</v>
+        <v>141</v>
       </c>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
@@ -4241,7 +4214,7 @@
         <v>2</v>
       </c>
       <c r="G70" s="10" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="H70" s="8">
         <v>0</v>
@@ -4256,7 +4229,7 @@
         <v>4.5</v>
       </c>
       <c r="L70" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="M70" s="8">
         <v>1</v>
@@ -4265,15 +4238,15 @@
         <v>3.25</v>
       </c>
       <c r="O70" s="11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="71" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
       <c r="A71" s="6" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
       <c r="B71" s="13"/>
-      <c r="C71" s="24"/>
+      <c r="C71" s="13"/>
       <c r="D71" s="8">
         <v>3</v>
       </c>
@@ -4284,7 +4257,7 @@
         <v>3</v>
       </c>
       <c r="G71" s="10" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="H71" s="14">
         <v>0</v>
@@ -4299,7 +4272,7 @@
         <v>3</v>
       </c>
       <c r="L71" s="10" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="M71" s="14">
         <v>0</v>
@@ -4308,12 +4281,12 @@
         <v>3</v>
       </c>
       <c r="O71" s="11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="72" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
       <c r="A72" s="6" t="s">
-        <v>116</v>
+        <v>143</v>
       </c>
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>
@@ -4327,7 +4300,7 @@
         <v>3</v>
       </c>
       <c r="G72" s="10" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="H72" s="8">
         <v>0</v>
@@ -4342,7 +4315,7 @@
         <v>3</v>
       </c>
       <c r="L72" s="10" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="M72" s="8">
         <v>0</v>
@@ -4351,12 +4324,12 @@
         <v>3</v>
       </c>
       <c r="O72" s="11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="73" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
       <c r="A73" s="15" t="s">
-        <v>117</v>
+        <v>144</v>
       </c>
       <c r="B73" s="7"/>
       <c r="C73" s="7"/>
@@ -4370,7 +4343,7 @@
         <v>2.5</v>
       </c>
       <c r="G73" s="10" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="H73" s="8">
         <v>0</v>
@@ -4385,7 +4358,7 @@
         <v>3</v>
       </c>
       <c r="L73" s="10" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="M73" s="8">
         <v>1</v>
@@ -4394,12 +4367,12 @@
         <v>2.75</v>
       </c>
       <c r="O73" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="74" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
       <c r="A74" s="6" t="s">
-        <v>118</v>
+        <v>145</v>
       </c>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
@@ -4413,7 +4386,7 @@
         <v>2.5</v>
       </c>
       <c r="G74" s="10" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="H74" s="8">
         <v>0</v>
@@ -4428,7 +4401,7 @@
         <v>2.5</v>
       </c>
       <c r="L74" s="10" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="M74" s="8">
         <v>0</v>
@@ -4437,12 +4410,12 @@
         <v>2.5</v>
       </c>
       <c r="O74" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="75" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
       <c r="A75" s="6" t="s">
-        <v>119</v>
+        <v>146</v>
       </c>
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
@@ -4456,7 +4429,7 @@
         <v>3</v>
       </c>
       <c r="G75" s="10" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="H75" s="8">
         <v>1</v>
@@ -4471,7 +4444,7 @@
         <v>1</v>
       </c>
       <c r="L75" s="10" t="s">
-        <v>120</v>
+        <v>147</v>
       </c>
       <c r="M75" s="8">
         <v>0</v>
@@ -4480,12 +4453,12 @@
         <v>2</v>
       </c>
       <c r="O75" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="76" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
       <c r="A76" s="6" t="s">
-        <v>121</v>
+        <v>148</v>
       </c>
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
@@ -4499,7 +4472,7 @@
         <v>2</v>
       </c>
       <c r="G76" s="10" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="H76" s="8">
         <v>0</v>
@@ -4514,7 +4487,7 @@
         <v>2</v>
       </c>
       <c r="L76" s="10" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="M76" s="8">
         <v>0</v>
@@ -4523,12 +4496,12 @@
         <v>2</v>
       </c>
       <c r="O76" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="77" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
       <c r="A77" s="6" t="s">
-        <v>122</v>
+        <v>149</v>
       </c>
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
@@ -4542,7 +4515,7 @@
         <v>2</v>
       </c>
       <c r="G77" s="10" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="H77" s="8">
         <v>0</v>
@@ -4557,7 +4530,7 @@
         <v>2</v>
       </c>
       <c r="L77" s="10" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="M77" s="8">
         <v>0</v>
@@ -4566,12 +4539,12 @@
         <v>2</v>
       </c>
       <c r="O77" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="78" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
       <c r="A78" s="6" t="s">
-        <v>123</v>
+        <v>150</v>
       </c>
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
@@ -4585,7 +4558,7 @@
         <v>2</v>
       </c>
       <c r="G78" s="10" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="H78" s="8">
         <v>0</v>
@@ -4600,7 +4573,7 @@
         <v>2</v>
       </c>
       <c r="L78" s="10" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="M78" s="8">
         <v>0</v>
@@ -4609,12 +4582,12 @@
         <v>2</v>
       </c>
       <c r="O78" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="79" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
       <c r="A79" s="6" t="s">
-        <v>124</v>
+        <v>151</v>
       </c>
       <c r="B79" s="7"/>
       <c r="C79" s="7"/>
@@ -4628,7 +4601,7 @@
         <v>2</v>
       </c>
       <c r="G79" s="10" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="H79" s="8">
         <v>0</v>
@@ -4643,7 +4616,7 @@
         <v>2</v>
       </c>
       <c r="L79" s="10" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="M79" s="8">
         <v>0</v>
@@ -4652,12 +4625,12 @@
         <v>2</v>
       </c>
       <c r="O79" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="80" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
       <c r="A80" s="6" t="s">
-        <v>125</v>
+        <v>152</v>
       </c>
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
@@ -4671,7 +4644,7 @@
         <v>1</v>
       </c>
       <c r="G80" s="10" t="s">
-        <v>120</v>
+        <v>147</v>
       </c>
       <c r="H80" s="8">
         <v>0</v>
@@ -4686,7 +4659,7 @@
         <v>2</v>
       </c>
       <c r="L80" s="10" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="M80" s="8">
         <v>1</v>
@@ -4695,12 +4668,12 @@
         <v>1.5</v>
       </c>
       <c r="O80" s="11" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="81" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
       <c r="A81" s="16" t="s">
-        <v>126</v>
+        <v>153</v>
       </c>
       <c r="B81" s="17"/>
       <c r="C81" s="17"/>
@@ -4714,7 +4687,7 @@
         <v>1</v>
       </c>
       <c r="G81" s="19" t="s">
-        <v>120</v>
+        <v>147</v>
       </c>
       <c r="H81" s="18">
         <v>0</v>
@@ -4729,7 +4702,7 @@
         <v>1</v>
       </c>
       <c r="L81" s="19" t="s">
-        <v>120</v>
+        <v>147</v>
       </c>
       <c r="M81" s="18">
         <v>0</v>
@@ -4738,7 +4711,7 @@
         <v>1</v>
       </c>
       <c r="O81" s="20" t="s">
-        <v>120</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>